<commit_message>
"Add ExcelOPerations for manipulating of excel sheets and commit for parameterizeTest update status col"
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/HalfTestData.xlsx
+++ b/src/test/java/testdata/HalfTestData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P52s-Workstation\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P52s-Workstation\IT Akademija vezbanje QA\java_programs\DDFSeleniumExcel\DDFSeleniumExcel\src\test\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCBA0FD-0DE2-407C-8CB4-D9D731380450}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EF8612-FF61-415B-9090-8AC5CEB3C5B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5556" xr2:uid="{E4A88FF8-C477-4616-97EC-921211741BB9}"/>
   </bookViews>
   <sheets>
     <sheet name="RegTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="HomePage" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>firstname</t>
   </si>
@@ -88,6 +89,12 @@
   </si>
   <si>
     <t>qwerty</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -140,13 +147,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -462,23 +470,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD587A3-8DAE-47C9-9FB0-BD7905574F21}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -497,8 +506,11 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -517,8 +529,11 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -537,8 +552,11 @@
       <c r="F3" s="3">
         <v>147852</v>
       </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -557,8 +575,11 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -576,6 +597,9 @@
       </c>
       <c r="F5" t="s">
         <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -589,4 +613,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
"DataProvider in TestNG. I add new test files HalfNGTest and testUtil for reading from excel sheets and creating object array for automation"
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/HalfTestData.xlsx
+++ b/src/test/java/testdata/HalfTestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P52s-Workstation\IT Akademija vezbanje QA\java_programs\DDFSeleniumExcel\DDFSeleniumExcel\src\test\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EF8612-FF61-415B-9090-8AC5CEB3C5B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F56048-40A7-4C33-AEDD-875657786E76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5556" xr2:uid="{E4A88FF8-C477-4616-97EC-921211741BB9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5556" activeTab="1" xr2:uid="{E4A88FF8-C477-4616-97EC-921211741BB9}"/>
   </bookViews>
   <sheets>
     <sheet name="RegTestData" sheetId="1" r:id="rId1"/>
-    <sheet name="HomePage" sheetId="3" r:id="rId2"/>
+    <sheet name="RegTestData2" sheetId="4" r:id="rId2"/>
+    <sheet name="HomePage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>firstname</t>
   </si>
@@ -95,13 +96,55 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>nic456@tgmail.com</t>
+  </si>
+  <si>
+    <t>Qwert123</t>
+  </si>
+  <si>
+    <t>Sdert123</t>
+  </si>
+  <si>
+    <t>Rwert123</t>
+  </si>
+  <si>
+    <t>Rert123</t>
+  </si>
+  <si>
+    <t>ni56@tgmail.com</t>
+  </si>
+  <si>
+    <t>kom56@tgmail.com</t>
+  </si>
+  <si>
+    <t>uio456@tgmail.com</t>
+  </si>
+  <si>
+    <t>Nikola</t>
+  </si>
+  <si>
+    <t>Vuk</t>
+  </si>
+  <si>
+    <t>Petrovic</t>
+  </si>
+  <si>
+    <t>Jovic</t>
+  </si>
+  <si>
+    <t>Badr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +168,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -155,6 +210,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -472,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD587A3-8DAE-47C9-9FB0-BD7905574F21}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -616,6 +672,105 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E826121-6D0F-4D65-8580-5BA470D2BE7A}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{8FF0CAC1-7FC3-41F5-A8E6-324644D222AA}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{DC1A4008-CA3E-4539-9BA7-BDA75E43D0DD}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{E4633567-2262-48DB-9A08-99EEB0C28004}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{E5F2B159-3FD7-49D5-8B1C-E0EB81D1EF90}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>